<commit_message>
updated country selection code with the last few changes from Anina
</commit_message>
<xml_diff>
--- a/data/gya-nations_look.xlsx
+++ b/data/gya-nations_look.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,8 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KristinaTietjen/Documents/Git_Hub/gya-research/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F614D5-E33C-BA4E-90EB-85EA2977C802}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2360" yWindow="460" windowWidth="23200" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="2360" yWindow="460" windowWidth="23200" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gya-nations_look" sheetId="1" r:id="rId1"/>
@@ -440,7 +441,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -450,7 +451,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -460,12 +461,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -482,10 +477,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -766,11 +760,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2915"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1794" sqref="F1794"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25045,30 +25039,30 @@
       </c>
     </row>
     <row r="1802" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1802" s="2" t="s">
+      <c r="A1802" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1802" s="2" t="s">
+      <c r="B1802" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1802" s="2" t="s">
+      <c r="C1802" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1802" s="2" t="s">
+      <c r="D1802" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="1803" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1803" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1803" s="2" t="s">
+      <c r="A1803" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1803" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1803" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1803" s="2" t="s">
+      <c r="C1803" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1803" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -25157,16 +25151,16 @@
       </c>
     </row>
     <row r="1810" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1810" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1810" s="2" t="s">
+      <c r="A1810" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1810" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1810" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1810" s="2" t="s">
+      <c r="C1810" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1810" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -25391,30 +25385,30 @@
       </c>
     </row>
     <row r="1828" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1828" s="2" t="s">
+      <c r="A1828" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B1828" s="2" t="s">
+      <c r="B1828" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1828" s="2" t="s">
+      <c r="C1828" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D1828" s="2" t="s">
+      <c r="D1828" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="1829" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1829" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1829" s="2" t="s">
+      <c r="A1829" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1829" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1829" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1829" s="2" t="s">
+      <c r="C1829" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1829" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -25567,16 +25561,16 @@
       </c>
     </row>
     <row r="1841" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1841" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1841" s="2" t="s">
+      <c r="A1841" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1841" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1841" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1841" s="2" t="s">
+      <c r="C1841" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1841" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -25631,16 +25625,16 @@
       </c>
     </row>
     <row r="1846" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1846" s="2" t="s">
+      <c r="A1846" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1846" s="2" t="s">
+      <c r="B1846" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1846" s="2" t="s">
+      <c r="C1846" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1846" s="2" t="s">
+      <c r="D1846" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -29213,16 +29207,16 @@
       </c>
     </row>
     <row r="2107" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2107" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2107" s="3" t="s">
+      <c r="A2107" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2107" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C2107" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2107" s="3" t="s">
+      <c r="C2107" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2107" s="2" t="s">
         <v>129</v>
       </c>
     </row>
@@ -29409,16 +29403,16 @@
       </c>
     </row>
     <row r="2121" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2121" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2121" s="3" t="s">
+      <c r="A2121" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2121" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C2121" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2121" s="3" t="s">
+      <c r="C2121" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2121" s="2" t="s">
         <v>129</v>
       </c>
     </row>
@@ -39169,16 +39163,16 @@
       </c>
     </row>
     <row r="2837" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2837" s="2" t="s">
+      <c r="A2837" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B2837" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2837" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2837" s="2" t="s">
+      <c r="B2837" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2837" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2837" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -39267,30 +39261,30 @@
       </c>
     </row>
     <row r="2844" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2844" s="2" t="s">
+      <c r="A2844" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B2844" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2844" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2844" s="2" t="s">
+      <c r="B2844" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2844" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2844" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2845" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2845" s="2" t="s">
+      <c r="A2845" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B2845" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2845" s="2" t="s">
+      <c r="B2845" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2845" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D2845" s="2" t="s">
+      <c r="D2845" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -39653,16 +39647,16 @@
       </c>
     </row>
     <row r="2872" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2872" s="2" t="s">
+      <c r="A2872" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B2872" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2872" s="2" t="s">
+      <c r="B2872" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2872" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D2872" s="2" t="s">
+      <c r="D2872" s="1" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>